<commit_message>
added in the sheets we need
</commit_message>
<xml_diff>
--- a/c_payment_token.xlsx
+++ b/c_payment_token.xlsx
@@ -509,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>2027.53</v>
+        <v>2064.03</v>
       </c>
     </row>
     <row r="3">
@@ -543,7 +543,7 @@
         <v>18</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0004932109512559617</v>
+        <v>0.0004844890820385362</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>2027.53</v>
+        <v>2064.03</v>
       </c>
     </row>
     <row r="5">
@@ -617,10 +617,10 @@
         <v>6</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0004930851824633914</v>
+        <v>0.0004842700929734548</v>
       </c>
       <c r="I5" t="n">
-        <v>0.999745</v>
+        <v>0.999548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>